<commit_message>
Update MO Hackathon - UncertainSea - Project Log.xlsx
test
</commit_message>
<xml_diff>
--- a/MO Hackathon - UncertainSea - Project Log.xlsx
+++ b/MO Hackathon - UncertainSea - Project Log.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perkinsth\Documents\Met Office Hackathon 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perkinsth\Documents\GitHub\UncertainSea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B944FD-3996-4E0C-A137-3D075A381382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DE71DB-1E0F-4041-9CC6-18F9177D17C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3D6C3FD5-F79E-43C8-B7E4-A5BABC36DA25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{3D6C3FD5-F79E-43C8-B7E4-A5BABC36DA25}"/>
   </bookViews>
   <sheets>
     <sheet name="Team list" sheetId="1" r:id="rId1"/>
     <sheet name="Data &amp; sources" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="121">
   <si>
     <t xml:space="preserve">Janet Peifer </t>
   </si>
@@ -401,6 +402,9 @@
   </si>
   <si>
     <t>Y?</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96997B0F-1B5E-426D-81B8-125FF74E6826}">
   <dimension ref="B1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1924,4 +1928,25 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <drawing r:id="rId14"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15420B46-6BBE-487A-9E50-C6DA9B7C7F74}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>